<commit_message>
Added a small set of example for URL Asset Import
</commit_message>
<xml_diff>
--- a/_acs-aem-commons/features/mcp-tools/asset-ingestion/url-asset-ingestor/url-asset-import-example.xlsx
+++ b/_acs-aem-commons/features/mcp-tools/asset-ingestion/url-asset-ingestor/url-asset-import-example.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB0A659-596F-4766-B26A-33FE1417BF67}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +19,135 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{947BD204-F865-44C6-BB6A-5F62BBE222DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+If you are not importing renditions and just assets you can remove C and D entirely.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Rendition</t>
+  </si>
+  <si>
+    <t>dc:description</t>
+  </si>
+  <si>
+    <t>cq:tags@[]</t>
+  </si>
+  <si>
+    <t>/content/dam/my-assets</t>
+  </si>
+  <si>
+    <t>http://www.boiledbeans.net/wp-content/uploads/2007/10/a4a5a0db727d718e645b845c462aed7f.jpg</t>
+  </si>
+  <si>
+    <t>Evil</t>
+  </si>
+  <si>
+    <t>Wikipedia-logo-v2.png</t>
+  </si>
+  <si>
+    <t>https://www.wikipedia.org/portal/wikipedia.org/assets/img/Wikipedia-logo-v2.png</t>
+  </si>
+  <si>
+    <t>Wikipedia logo</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>This column is totally ignored and is here for human purposes</t>
+  </si>
+  <si>
+    <t>This is added as a rendition to the first image above, it has no metadata of its own</t>
+  </si>
+  <si>
+    <t>This is ignored</t>
+  </si>
+  <si>
+    <t>This is ignored.</t>
+  </si>
+  <si>
+    <t>http://www.iamwire.com/wp-content/uploads/2017/08/colour-logo.jpg</t>
+  </si>
+  <si>
+    <t>/content/dam/my-assets/logos</t>
+  </si>
+  <si>
+    <t>http://www.iamwire.com/wp-content/uploads/2017/08/logo-design.jpg</t>
+  </si>
+  <si>
+    <t>http://www.iamwire.com/wp-content/uploads/2017/08/famous_shapes.jpg</t>
+  </si>
+  <si>
+    <t>http-bad-protocol://www.nowhere.com/some-image.jpg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/static/images/project-logos/enwiki-2x.png-404-error</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org.dns.error/static/images/project-logos/enwiki-2x.png</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/static/images/project-logos/enwiki-2x spaces not allowed.png</t>
+  </si>
+  <si>
+    <t>Should fail because the URL is invalid</t>
+  </si>
+  <si>
+    <t>Should fail with a 404 error</t>
+  </si>
+  <si>
+    <t>Should fail because the URL is incorrect (bad host name)</t>
+  </si>
+  <si>
+    <t>Should fail because URLs shouldn't have spaces in them</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +155,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +208,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +497,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="83.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.53125" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.06640625" customWidth="1"/>
+    <col min="6" max="6" width="28.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BB5F944D-1F35-44BD-82CF-1DCBD2702ADC}"/>
+    <hyperlink ref="A8" r:id="rId2" xr:uid="{CE117BDC-E993-40C3-9FD8-11D27A7108E6}"/>
+    <hyperlink ref="A9" r:id="rId3" xr:uid="{0DE6894E-4A63-4061-8B77-4A8792696BEA}"/>
+    <hyperlink ref="A10" r:id="rId4" xr:uid="{C09D1448-9F90-49C4-975D-7B1CFA4A13DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated example to add a couple of tags.
</commit_message>
<xml_diff>
--- a/_acs-aem-commons/features/mcp-tools/asset-ingestion/url-asset-ingestor/url-asset-import-example.xlsx
+++ b/_acs-aem-commons/features/mcp-tools/asset-ingestion/url-asset-ingestor/url-asset-import-example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB0A659-596F-4766-B26A-33FE1417BF67}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295B4ADF-2632-4BF0-9934-313E9803DD53}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Source</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Should fail because URLs shouldn't have spaces in them</t>
+  </si>
+  <si>
+    <t>properties:orientation/square</t>
+  </si>
+  <si>
+    <t>properties:orientation/landscape,properties:style/color</t>
+  </si>
+  <si>
+    <t>properties:orientation/landscape,properties:style/monochrome</t>
   </si>
 </sst>
 </file>
@@ -212,11 +221,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -511,7 +523,7 @@
     <col min="3" max="3" width="14.53125" customWidth="1"/>
     <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.06640625" customWidth="1"/>
-    <col min="6" max="6" width="28.73046875" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -547,6 +559,9 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
@@ -574,28 +589,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>